<commit_message>
cambios QoL para errores
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\IdeaProjects\Asitente_Inclusiones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\oscortes12\ProjectsData\IdeaProjects\PROYINCLUSIONES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0FA03F-81C2-4425-93ED-9C1E194010C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2581683-09A9-418C-AE3D-99F04523C337}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-840" yWindow="3216" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22350" yWindow="2595" windowWidth="15480" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan 2050" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="198">
   <si>
     <t>Creditos</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Semestre</t>
   </si>
   <si>
-    <t>CI0200</t>
-  </si>
-  <si>
     <t>CI0202</t>
   </si>
   <si>
@@ -443,13 +440,181 @@
     <t>CI1403,FH1000,SE1100,SE1200,SE1400,TI4101,TI5000,TI6000,TI6502,TI7102,TI9003,TI9004,TI9005,TI9006,TI9804,TI9805,TI9905</t>
   </si>
   <si>
-    <t>Nada</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nuevo</t>
-  </si>
-  <si>
-    <t>nada</t>
+    <t>COMUNICACION ESCRITA</t>
+  </si>
+  <si>
+    <t>MODELOS ORGANIZACIONALES Y GESTION DE TI</t>
+  </si>
+  <si>
+    <t>TI1103</t>
+  </si>
+  <si>
+    <t>CALCULO DIFERENCIAL E INTEGRAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ORGANIZACION Y ARQUITECTURA DE COMPUTADORES</t>
+  </si>
+  <si>
+    <t>TI2404</t>
+  </si>
+  <si>
+    <t>INGENIERIA DE REQUERIMIENTOS</t>
+  </si>
+  <si>
+    <t>T11400</t>
+  </si>
+  <si>
+    <t>TI1201</t>
+  </si>
+  <si>
+    <t>COMPORTAMIENTO ORGANIZACIONAL Y TALENTO HUMANO</t>
+  </si>
+  <si>
+    <t>MA1402</t>
+  </si>
+  <si>
+    <t>COMUNICACION ORAL</t>
+  </si>
+  <si>
+    <t>CI1107</t>
+  </si>
+  <si>
+    <t>CALCULO Y ALGEBRA LINEAL</t>
+  </si>
+  <si>
+    <t>MA1103</t>
+  </si>
+  <si>
+    <t>TI2201</t>
+  </si>
+  <si>
+    <t>PROGRAMACION ORIENTADA A OBJETOS</t>
+  </si>
+  <si>
+    <t>TI4500,TI2201</t>
+  </si>
+  <si>
+    <t>T13501</t>
+  </si>
+  <si>
+    <t>FUNDAMENTOS DE SISTEMAS OPERATIVOS</t>
+  </si>
+  <si>
+    <t>T12404</t>
+  </si>
+  <si>
+    <t>TI4200, TI4101</t>
+  </si>
+  <si>
+    <t>TI3500</t>
+  </si>
+  <si>
+    <t>MERCADEO EN LA ERA DIGITAL</t>
+  </si>
+  <si>
+    <t>CS3404</t>
+  </si>
+  <si>
+    <t>SEMINARIO DE ETICA PARA LA INGENIERIA</t>
+  </si>
+  <si>
+    <t>TI3603</t>
+  </si>
+  <si>
+    <t>CALIDAD EN SISTEMAS DE INFORMACION</t>
+  </si>
+  <si>
+    <t>TI5501, TI3801</t>
+  </si>
+  <si>
+    <t>TI3604</t>
+  </si>
+  <si>
+    <t>FUNDAMENTOS DE REDES</t>
+  </si>
+  <si>
+    <t>TI3602</t>
+  </si>
+  <si>
+    <t>DERECHO LABORAL</t>
+  </si>
+  <si>
+    <t>CS2304</t>
+  </si>
+  <si>
+    <t>CS3403, TI1201</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA DE APLICACIONES</t>
+  </si>
+  <si>
+    <t>TI4701</t>
+  </si>
+  <si>
+    <t>SEGURIDAD EN SISTEMAS DE INFORMACION</t>
+  </si>
+  <si>
+    <t>NEGOCIOS ELECTRONICOS</t>
+  </si>
+  <si>
+    <t>TI3603, TI6900</t>
+  </si>
+  <si>
+    <t>TI6101,TI3500</t>
+  </si>
+  <si>
+    <t>CS3405</t>
+  </si>
+  <si>
+    <t>DERECHO INFORMATICO Y MERCANTIL</t>
+  </si>
+  <si>
+    <t>TI6703, TI8109</t>
+  </si>
+  <si>
+    <t>INVESTIGACION EN SISTEMAS DE INFORMACION</t>
+  </si>
+  <si>
+    <t>TI8904, TI9905</t>
+  </si>
+  <si>
+    <t>TI5904</t>
+  </si>
+  <si>
+    <t>TI5905</t>
+  </si>
+  <si>
+    <t>FUNDAMENTOS DE ARQUITECTURA EMPRESARIAL</t>
+  </si>
+  <si>
+    <t>TI5903</t>
+  </si>
+  <si>
+    <t>PLANIFICACION ESTRATEGICA DE TECNOLOGIA DE INFORMACION</t>
+  </si>
+  <si>
+    <t>TI5902</t>
+  </si>
+  <si>
+    <t>ANALITICA EMPRESARIAL</t>
+  </si>
+  <si>
+    <t>TI5901</t>
+  </si>
+  <si>
+    <t>TI5904,TI5905,TI5903,TI5902, TI9004,TI5901</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INFORMACION CONTABLE</t>
+  </si>
+  <si>
+    <t>TI1102</t>
+  </si>
+  <si>
+    <t>CI1106</t>
+  </si>
+  <si>
+    <t>TI3601</t>
   </si>
 </sst>
 </file>
@@ -946,48 +1111,48 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1003,7 +1168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1299,15 +1464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1321,32 +1486,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1355,69 +1514,69 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1426,12 +1585,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1440,886 +1599,872 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="F25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>41</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
       </c>
       <c r="F26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="F29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32">
         <v>4</v>
       </c>
-      <c r="D31" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F32">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F33">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F34">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F35">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="F36">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="F37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F38">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F39">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F40">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F41">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C42">
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F42">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F43">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C44">
         <v>3</v>
-      </c>
-      <c r="D44" t="s">
-        <v>75</v>
       </c>
       <c r="F44">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C45">
         <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>74</v>
       </c>
       <c r="F45">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="F46">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F47">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C48">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="F48">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C49">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="F49">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C50">
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="F50">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F51">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="F52">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F53">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="F54">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C55">
         <v>3</v>
       </c>
-      <c r="D55" t="s">
-        <v>108</v>
-      </c>
       <c r="F55">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B56" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C56">
         <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>116</v>
       </c>
       <c r="F56">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B57" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C57">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F57">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="F58">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B59" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C59">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F59">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B60" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F60">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C61">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="F61">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>137</v>
-      </c>
-      <c r="B62" t="s">
-        <v>138</v>
-      </c>
-      <c r="C62">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>139</v>
-      </c>
-      <c r="F62">
         <v>10</v>
       </c>
     </row>
@@ -2331,15 +2476,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052F1038-1236-4088-917B-55AEDD879593}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -2353,32 +2503,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" t="s">
-        <v>142</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2387,972 +2531,990 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>194</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>139</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>143</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>19</v>
+      <c r="D11" t="s">
+        <v>20</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>145</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>146</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>148</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>141</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18">
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D23" t="s">
         <v>40</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>43</v>
       </c>
-      <c r="C20">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>50</v>
-      </c>
-      <c r="F23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
       </c>
       <c r="F26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
         <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="F29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="F30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
       <c r="F31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="F32">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="F33">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F34">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="F35">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="F36">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>167</v>
       </c>
       <c r="F37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="F38">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F39">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" t="s">
         <v>87</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
         <v>88</v>
-      </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>89</v>
       </c>
       <c r="F40">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>197</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F41">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="F42">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
       <c r="F43">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
       <c r="C44">
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="F44">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>175</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
       <c r="C45">
         <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>168</v>
       </c>
       <c r="F45">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>177</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="F46">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C47">
         <v>3</v>
-      </c>
-      <c r="D47" t="s">
-        <v>104</v>
       </c>
       <c r="F47">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C48">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="F48">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>181</v>
       </c>
       <c r="C49">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="F49">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="C50">
-        <v>3</v>
-      </c>
-      <c r="D50" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F51">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="F52">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C53">
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="F53">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="F54">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C55">
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F55">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" t="s">
         <v>125</v>
       </c>
-      <c r="B56" t="s">
-        <v>126</v>
-      </c>
       <c r="C56">
         <v>3</v>
       </c>
       <c r="F56">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="B57" t="s">
-        <v>128</v>
+        <v>183</v>
       </c>
       <c r="C57">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="F57">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
       <c r="B58" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>110</v>
+        <v>186</v>
       </c>
       <c r="F58">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="B59" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="C59">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F59">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="B60" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
         <v>134</v>
-      </c>
-      <c r="C60">
-        <v>3</v>
-      </c>
-      <c r="D60" t="s">
-        <v>113</v>
       </c>
       <c r="F60">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F61">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" t="s">
         <v>137</v>
       </c>
-      <c r="B62" t="s">
-        <v>138</v>
-      </c>
-      <c r="C62">
+      <c r="C63">
         <v>10</v>
       </c>
-      <c r="D62" t="s">
-        <v>139</v>
-      </c>
-      <c r="F62">
+      <c r="D63" t="s">
+        <v>193</v>
+      </c>
+      <c r="F63">
         <v>10</v>
       </c>
     </row>

</xml_diff>